<commit_message>
completed stat analysis of black hispanic vs white for arrests and force
</commit_message>
<xml_diff>
--- a/significance_analysis.xlsx
+++ b/significance_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tielqueen/Google Drive/SENIOR YEAR!/Winter Quarter/CS191/cpz_ripa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF14929D-669D-0D40-8912-D071DE655563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A9CEF7-2B8E-BC41-AA15-3B32859214CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16720" xr2:uid="{AF49FA5B-4AFB-F346-B8F7-A6A43AD9202B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="15">
   <si>
     <t>Agency</t>
   </si>
@@ -119,10 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,23 +438,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87903FE-6F12-B049-9B24-BAF57835F691}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -463,19 +468,37 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>1.0100000000000001E-174</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2.4300000000000002E-212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -485,8 +508,17 @@
       <c r="C4" s="2">
         <v>4.9100000000000004E-152</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5.6100000000000004E-165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -496,8 +528,17 @@
       <c r="C5" s="2">
         <v>1.8400000000000002E-176</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6.1599999999999997E-173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -507,8 +548,17 @@
       <c r="C6" s="2">
         <v>1.9899999999999999E-280</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4.66E-180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -518,8 +568,17 @@
       <c r="C7" s="2">
         <v>1.1099999999999999E-258</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9.2999999999999996E-232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -529,8 +588,17 @@
       <c r="C8" s="2">
         <v>1.77E-202</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5.81E-196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -540,8 +608,17 @@
       <c r="C9" s="2">
         <v>7.4900000000000005E-203</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2.8199999999999998E-175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -551,8 +628,17 @@
       <c r="C10" s="2">
         <v>1.2500000000000001E-216</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.5600000000000002E-209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -562,8 +648,17 @@
       <c r="C11" s="2">
         <v>6.1899999999999999E-147</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.06E-140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -573,8 +668,17 @@
       <c r="C12" s="2">
         <v>3.9000000000000001E-129</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.15E-146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -584,8 +688,17 @@
       <c r="C13" s="2">
         <v>1.8500000000000001E-180</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3.6799999999999999E-140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -595,8 +708,17 @@
       <c r="C14" s="2">
         <v>3.9200000000000001E-143</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2">
+        <v>7.1499999999999997E-227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -606,8 +728,17 @@
       <c r="C15" s="2">
         <v>8.68E-193</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.09E-168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -617,8 +748,17 @@
       <c r="C16" s="2">
         <v>9.8500000000000006E-142</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3.2200000000000001E-131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -628,8 +768,17 @@
       <c r="C17" s="2">
         <v>3.4500000000000001E-235</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2">
+        <v>6.1700000000000005E-224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -639,10 +788,14 @@
       <c r="C18" s="2">
         <v>8.4300000000000001E-172</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3.4499999999999999E-143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>